<commit_message>
include urls from wikidata
</commit_message>
<xml_diff>
--- a/data/refine_all.xlsx
+++ b/data/refine_all.xlsx
@@ -585,10 +585,10 @@
     <t>RDA Europe (Nodes)</t>
   </si>
   <si>
-    <t>Riina Salmivalli</t>
-  </si>
-  <si>
-    <t>riina.salmivalli@csc.fi</t>
+    <t>Irina Kupiainen</t>
+  </si>
+  <si>
+    <t>irina.kupiainen@csc.fi</t>
   </si>
   <si>
     <t>grid.452089.2</t>
@@ -3166,10 +3166,10 @@
       <c r="C31" t="s">
         <v>189</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="1" t="s">
         <v>191</v>
       </c>
       <c r="J31" t="s">

</xml_diff>

<commit_message>
fix some names and destinations
</commit_message>
<xml_diff>
--- a/data/refine_all.xlsx
+++ b/data/refine_all.xlsx
@@ -2013,7 +2013,7 @@
     <t>Q6269240</t>
   </si>
   <si>
-    <t>Franck Manista</t>
+    <t>Frank Manista</t>
   </si>
   <si>
     <t>frank.manista@jisc.ac.uk</t>
@@ -4902,7 +4902,7 @@
         <v>52.3567326</v>
       </c>
       <c r="O83" s="1">
-        <v>49.524732</v>
+        <v>4.9524732</v>
       </c>
     </row>
     <row r="84" ht="15.75" customHeight="1">
@@ -4936,11 +4936,11 @@
       <c r="M84" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="N84" s="1">
-        <v>52.0890599</v>
-      </c>
-      <c r="O84" s="1">
-        <v>51.112714</v>
+      <c r="N84" s="2">
+        <v>52.089151</v>
+      </c>
+      <c r="O84" s="2">
+        <v>5.113453</v>
       </c>
     </row>
     <row r="85" ht="15.75" customHeight="1">
@@ -6093,7 +6093,7 @@
       <c r="C121" t="s">
         <v>17</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D121" s="1" t="s">
         <v>666</v>
       </c>
       <c r="E121" t="s">
@@ -6206,10 +6206,10 @@
         <v>670</v>
       </c>
       <c r="N124" s="1">
-        <v>51.5237868</v>
+        <v>51.52399</v>
       </c>
       <c r="O124" s="1">
-        <v>-4.23039</v>
+        <v>-0.0423039</v>
       </c>
     </row>
     <row r="125" hidden="1"/>

</xml_diff>